<commit_message>
* smaller fixes in kjp generator
</commit_message>
<xml_diff>
--- a/backend/data/excel/KJPListe.xlsx
+++ b/backend/data/excel/KJPListe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philip/PycharmProjects/anmelde-tool/backend/data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62F2AC0-1172-1641-970E-6EF45AD583A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE11864-1CC7-6241-86C5-A2689B479470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -290,9 +290,6 @@
     <t/>
   </si>
   <si>
-    <t>/ 1</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -303,6 +300,9 @@
   </si>
   <si>
     <t>Robert-Perthel-Str. 79, 50739 Köln</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
@@ -994,9 +994,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1023,6 +1020,354 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="5" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="5" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="5" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="5" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="5" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="5" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="5" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="5" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="5" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="5" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="5" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="5" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="5" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="5" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1032,6 +1377,9 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="3" fontId="8" fillId="5" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="8" fillId="5" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1041,24 +1389,6 @@
     <xf numFmtId="3" fontId="8" fillId="5" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="5" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="5" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1071,350 +1401,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="5" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="5" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="5" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="5" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="5" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="5" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="5" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="5" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="5" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="5" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="5" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="5" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="5" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2271,9 +2271,7 @@
           </cell>
         </row>
         <row r="3">
-          <cell r="A3" t="str">
-            <v/>
-          </cell>
+          <cell r="A3"/>
           <cell r="G3">
             <v>1</v>
           </cell>
@@ -2300,32 +2298,16 @@
           <cell r="B4">
             <v>0</v>
           </cell>
-          <cell r="G4" t="str">
-            <v/>
-          </cell>
-          <cell r="H4" t="str">
-            <v/>
-          </cell>
-          <cell r="I4" t="str">
-            <v/>
-          </cell>
-          <cell r="J4" t="str">
-            <v/>
-          </cell>
-          <cell r="K4" t="str">
-            <v/>
-          </cell>
-          <cell r="L4" t="str">
-            <v/>
-          </cell>
+          <cell r="G4"/>
+          <cell r="H4"/>
+          <cell r="I4"/>
+          <cell r="J4"/>
+          <cell r="K4"/>
+          <cell r="L4"/>
         </row>
         <row r="5">
-          <cell r="A5" t="str">
-            <v/>
-          </cell>
-          <cell r="B5" t="str">
-            <v/>
-          </cell>
+          <cell r="A5"/>
+          <cell r="B5"/>
         </row>
         <row r="6">
           <cell r="A6" t="str">
@@ -2354,9 +2336,7 @@
           </cell>
         </row>
         <row r="7">
-          <cell r="A7" t="str">
-            <v/>
-          </cell>
+          <cell r="A7"/>
           <cell r="E7" t="str">
             <v>Position auf TN-Liste</v>
           </cell>
@@ -2383,38 +2363,20 @@
           <cell r="F8" t="str">
             <v>Lfd.-Nr.</v>
           </cell>
-          <cell r="G8" t="str">
-            <v/>
-          </cell>
-          <cell r="H8" t="str">
-            <v/>
-          </cell>
-          <cell r="I8" t="str">
-            <v/>
-          </cell>
-          <cell r="J8" t="str">
-            <v/>
-          </cell>
-          <cell r="K8" t="str">
-            <v/>
-          </cell>
-          <cell r="L8" t="str">
-            <v/>
-          </cell>
+          <cell r="G8"/>
+          <cell r="H8"/>
+          <cell r="I8"/>
+          <cell r="J8"/>
+          <cell r="K8"/>
+          <cell r="L8"/>
         </row>
         <row r="9">
           <cell r="A9" t="str">
             <v>...noch keine Inhalte in KÜ (intern)</v>
           </cell>
-          <cell r="E9" t="str">
-            <v/>
-          </cell>
-          <cell r="G9" t="str">
-            <v/>
-          </cell>
-          <cell r="H9" t="str">
-            <v/>
-          </cell>
+          <cell r="E9"/>
+          <cell r="G9"/>
+          <cell r="H9"/>
         </row>
       </sheetData>
       <sheetData sheetId="5"/>
@@ -2731,7 +2693,7 @@
   <dimension ref="A1:BD32"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="V25" sqref="V25:Y25"/>
+      <selection activeCell="AH29" sqref="AH29:BC31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="13"/>
@@ -2747,8 +2709,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55">
-      <c r="A1" s="93"/>
-      <c r="B1" s="92"/>
+      <c r="A1" s="92"/>
+      <c r="B1" s="91"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
@@ -2764,19 +2726,19 @@
       <c r="O1" s="49"/>
       <c r="P1" s="49"/>
       <c r="Q1" s="49"/>
-      <c r="R1" s="91"/>
+      <c r="R1" s="90"/>
       <c r="S1" s="49"/>
-      <c r="T1" s="91" t="s">
+      <c r="T1" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="U1" s="186">
-        <v>0</v>
-      </c>
-      <c r="V1" s="186"/>
-      <c r="W1" s="90"/>
+      <c r="U1" s="93">
+        <v>44562</v>
+      </c>
+      <c r="V1" s="93"/>
+      <c r="W1" s="89"/>
       <c r="X1" s="49"/>
-      <c r="Y1" s="90"/>
-      <c r="Z1" s="90"/>
+      <c r="Y1" s="89"/>
+      <c r="Z1" s="89"/>
       <c r="AA1" s="49"/>
       <c r="AB1" s="49"/>
       <c r="AC1" s="49"/>
@@ -2788,19 +2750,19 @@
       <c r="AI1" s="47"/>
       <c r="AJ1" s="47"/>
       <c r="AK1" s="47"/>
-      <c r="AL1" s="89"/>
+      <c r="AL1" s="88"/>
       <c r="AM1" s="47"/>
       <c r="AN1" s="47"/>
       <c r="AO1" s="47"/>
       <c r="AP1" s="47"/>
-      <c r="AQ1" s="88" t="s">
+      <c r="AQ1" s="87" t="s">
         <v>0</v>
       </c>
       <c r="AR1" s="47"/>
-      <c r="AS1" s="87" t="s">
+      <c r="AS1" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="AT1" s="87"/>
+      <c r="AT1" s="86"/>
       <c r="AU1" s="47"/>
       <c r="AV1" s="47"/>
       <c r="AW1" s="47"/>
@@ -2812,11 +2774,11 @@
       <c r="BC1" s="46"/>
     </row>
     <row r="2" spans="1:55">
-      <c r="A2" s="86"/>
+      <c r="A2" s="85"/>
       <c r="BC2" s="34"/>
     </row>
     <row r="3" spans="1:55" ht="14" thickBot="1">
-      <c r="A3" s="85"/>
+      <c r="A3" s="84"/>
       <c r="B3" s="54"/>
       <c r="C3" s="54"/>
       <c r="D3" s="54"/>
@@ -2839,8 +2801,8 @@
       <c r="U3" s="54"/>
       <c r="V3" s="54"/>
       <c r="W3" s="54"/>
-      <c r="X3" s="84"/>
-      <c r="Y3" s="84"/>
+      <c r="X3" s="83"/>
+      <c r="Y3" s="83"/>
       <c r="Z3" s="54"/>
       <c r="AA3" s="54"/>
       <c r="AB3" s="54"/>
@@ -2864,21 +2826,23 @@
       <c r="AT3" s="54"/>
       <c r="AU3" s="54"/>
       <c r="AV3" s="54"/>
-      <c r="AW3" s="83" t="s">
+      <c r="AW3" s="82" t="s">
         <v>61</v>
       </c>
       <c r="AX3" s="54"/>
-      <c r="AY3" s="82" t="s">
+      <c r="AY3" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="AZ3" s="81">
+      <c r="AZ3" s="80">
         <v>1</v>
       </c>
-      <c r="BA3" s="80"/>
-      <c r="BB3" s="178" t="s">
-        <v>62</v>
-      </c>
-      <c r="BC3" s="179"/>
+      <c r="BA3" s="223" t="s">
+        <v>66</v>
+      </c>
+      <c r="BB3" s="134">
+        <v>1</v>
+      </c>
+      <c r="BC3" s="135"/>
     </row>
     <row r="4" spans="1:55">
       <c r="A4" s="79" t="s">
@@ -2942,48 +2906,48 @@
       <c r="BC4" s="46"/>
     </row>
     <row r="5" spans="1:55">
-      <c r="A5" s="122"/>
-      <c r="B5" s="221"/>
-      <c r="C5" s="221"/>
-      <c r="D5" s="221"/>
-      <c r="E5" s="221"/>
-      <c r="F5" s="221"/>
-      <c r="G5" s="221"/>
-      <c r="H5" s="221"/>
-      <c r="I5" s="221"/>
-      <c r="J5" s="221"/>
-      <c r="K5" s="221"/>
-      <c r="L5" s="221"/>
-      <c r="M5" s="221"/>
-      <c r="N5" s="221"/>
-      <c r="O5" s="221"/>
-      <c r="P5" s="221"/>
-      <c r="Q5" s="221"/>
-      <c r="R5" s="221"/>
-      <c r="S5" s="221"/>
-      <c r="T5" s="221"/>
-      <c r="U5" s="221"/>
-      <c r="V5" s="221"/>
-      <c r="W5" s="221"/>
-      <c r="X5" s="221"/>
-      <c r="Y5" s="221"/>
-      <c r="Z5" s="123"/>
-      <c r="AA5" s="187" t="s">
+      <c r="A5" s="128"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="129"/>
+      <c r="L5" s="129"/>
+      <c r="M5" s="129"/>
+      <c r="N5" s="129"/>
+      <c r="O5" s="129"/>
+      <c r="P5" s="129"/>
+      <c r="Q5" s="129"/>
+      <c r="R5" s="129"/>
+      <c r="S5" s="129"/>
+      <c r="T5" s="129"/>
+      <c r="U5" s="129"/>
+      <c r="V5" s="129"/>
+      <c r="W5" s="129"/>
+      <c r="X5" s="129"/>
+      <c r="Y5" s="129"/>
+      <c r="Z5" s="130"/>
+      <c r="AA5" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="AB5" s="188"/>
-      <c r="AC5" s="188"/>
-      <c r="AD5" s="188"/>
-      <c r="AE5" s="188"/>
-      <c r="AF5" s="188"/>
-      <c r="AG5" s="188"/>
-      <c r="AH5" s="188"/>
-      <c r="AI5" s="188"/>
-      <c r="AJ5" s="188"/>
-      <c r="AK5" s="188"/>
-      <c r="AL5" s="188"/>
-      <c r="AM5" s="188"/>
-      <c r="AN5" s="188"/>
+      <c r="AB5" s="95"/>
+      <c r="AC5" s="95"/>
+      <c r="AD5" s="95"/>
+      <c r="AE5" s="95"/>
+      <c r="AF5" s="95"/>
+      <c r="AG5" s="95"/>
+      <c r="AH5" s="95"/>
+      <c r="AI5" s="95"/>
+      <c r="AJ5" s="95"/>
+      <c r="AK5" s="95"/>
+      <c r="AL5" s="95"/>
+      <c r="AM5" s="95"/>
+      <c r="AN5" s="95"/>
       <c r="AT5" s="77"/>
       <c r="AU5" s="76" t="s">
         <v>6</v>
@@ -2994,48 +2958,48 @@
       <c r="BC5" s="34"/>
     </row>
     <row r="6" spans="1:55">
-      <c r="A6" s="125" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="126"/>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="126"/>
-      <c r="N6" s="126"/>
-      <c r="O6" s="126"/>
-      <c r="P6" s="126"/>
-      <c r="Q6" s="126"/>
-      <c r="R6" s="126"/>
-      <c r="S6" s="126"/>
-      <c r="T6" s="126"/>
-      <c r="U6" s="126"/>
-      <c r="V6" s="126"/>
-      <c r="W6" s="126"/>
-      <c r="X6" s="126"/>
-      <c r="Y6" s="126"/>
-      <c r="Z6" s="127"/>
-      <c r="AA6" s="187"/>
-      <c r="AB6" s="188"/>
-      <c r="AC6" s="188"/>
-      <c r="AD6" s="188"/>
-      <c r="AE6" s="188"/>
-      <c r="AF6" s="188"/>
-      <c r="AG6" s="188"/>
-      <c r="AH6" s="188"/>
-      <c r="AI6" s="188"/>
-      <c r="AJ6" s="188"/>
-      <c r="AK6" s="188"/>
-      <c r="AL6" s="188"/>
-      <c r="AM6" s="188"/>
-      <c r="AN6" s="188"/>
+      <c r="A6" s="131" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="132"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="132"/>
+      <c r="Q6" s="132"/>
+      <c r="R6" s="132"/>
+      <c r="S6" s="132"/>
+      <c r="T6" s="132"/>
+      <c r="U6" s="132"/>
+      <c r="V6" s="132"/>
+      <c r="W6" s="132"/>
+      <c r="X6" s="132"/>
+      <c r="Y6" s="132"/>
+      <c r="Z6" s="133"/>
+      <c r="AA6" s="94"/>
+      <c r="AB6" s="95"/>
+      <c r="AC6" s="95"/>
+      <c r="AD6" s="95"/>
+      <c r="AE6" s="95"/>
+      <c r="AF6" s="95"/>
+      <c r="AG6" s="95"/>
+      <c r="AH6" s="95"/>
+      <c r="AI6" s="95"/>
+      <c r="AJ6" s="95"/>
+      <c r="AK6" s="95"/>
+      <c r="AL6" s="95"/>
+      <c r="AM6" s="95"/>
+      <c r="AN6" s="95"/>
       <c r="AT6" s="74"/>
       <c r="AU6" s="73" t="s">
         <v>8</v>
@@ -3050,34 +3014,34 @@
       <c r="BC6" s="70"/>
     </row>
     <row r="7" spans="1:55">
-      <c r="A7" s="125" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="126"/>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="126"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="126"/>
-      <c r="N7" s="126"/>
-      <c r="O7" s="126"/>
-      <c r="P7" s="126"/>
-      <c r="Q7" s="126"/>
-      <c r="R7" s="126"/>
-      <c r="S7" s="126"/>
-      <c r="T7" s="126"/>
-      <c r="U7" s="126"/>
-      <c r="V7" s="126"/>
-      <c r="W7" s="126"/>
-      <c r="X7" s="126"/>
-      <c r="Y7" s="126"/>
-      <c r="Z7" s="127"/>
+      <c r="A7" s="131" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="132"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="132"/>
+      <c r="H7" s="132"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="132"/>
+      <c r="K7" s="132"/>
+      <c r="L7" s="132"/>
+      <c r="M7" s="132"/>
+      <c r="N7" s="132"/>
+      <c r="O7" s="132"/>
+      <c r="P7" s="132"/>
+      <c r="Q7" s="132"/>
+      <c r="R7" s="132"/>
+      <c r="S7" s="132"/>
+      <c r="T7" s="132"/>
+      <c r="U7" s="132"/>
+      <c r="V7" s="132"/>
+      <c r="W7" s="132"/>
+      <c r="X7" s="132"/>
+      <c r="Y7" s="132"/>
+      <c r="Z7" s="133"/>
       <c r="AA7" s="35" t="s">
         <v>9</v>
       </c>
@@ -3088,83 +3052,83 @@
       <c r="BC7" s="34"/>
     </row>
     <row r="8" spans="1:55">
-      <c r="A8" s="125" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="126"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="126"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="126"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
-      <c r="J8" s="126"/>
-      <c r="K8" s="126"/>
-      <c r="L8" s="126"/>
-      <c r="M8" s="126"/>
-      <c r="N8" s="126"/>
-      <c r="O8" s="126"/>
-      <c r="P8" s="126"/>
-      <c r="Q8" s="126"/>
-      <c r="R8" s="126"/>
-      <c r="S8" s="126"/>
-      <c r="T8" s="126"/>
-      <c r="U8" s="126"/>
-      <c r="V8" s="126"/>
-      <c r="W8" s="126"/>
-      <c r="X8" s="126"/>
-      <c r="Y8" s="126"/>
-      <c r="Z8" s="127"/>
+      <c r="A8" s="131" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
+      <c r="H8" s="132"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
+      <c r="K8" s="132"/>
+      <c r="L8" s="132"/>
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="132"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="132"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="132"/>
+      <c r="X8" s="132"/>
+      <c r="Y8" s="132"/>
+      <c r="Z8" s="133"/>
       <c r="AA8" s="35" t="s">
         <v>10</v>
       </c>
       <c r="AI8" s="3"/>
-      <c r="AO8" s="189" t="s">
+      <c r="AO8" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="AP8" s="190"/>
-      <c r="AQ8" s="190"/>
-      <c r="AR8" s="190"/>
-      <c r="AS8" s="190"/>
-      <c r="AT8" s="190"/>
-      <c r="AU8" s="190"/>
-      <c r="AV8" s="190"/>
-      <c r="AW8" s="190"/>
-      <c r="AX8" s="190"/>
-      <c r="AY8" s="190"/>
-      <c r="AZ8" s="190"/>
-      <c r="BA8" s="190"/>
-      <c r="BB8" s="190"/>
-      <c r="BC8" s="191"/>
+      <c r="AP8" s="97"/>
+      <c r="AQ8" s="97"/>
+      <c r="AR8" s="97"/>
+      <c r="AS8" s="97"/>
+      <c r="AT8" s="97"/>
+      <c r="AU8" s="97"/>
+      <c r="AV8" s="97"/>
+      <c r="AW8" s="97"/>
+      <c r="AX8" s="97"/>
+      <c r="AY8" s="97"/>
+      <c r="AZ8" s="97"/>
+      <c r="BA8" s="97"/>
+      <c r="BB8" s="97"/>
+      <c r="BC8" s="98"/>
     </row>
     <row r="9" spans="1:55" ht="14" thickBot="1">
-      <c r="A9" s="128"/>
-      <c r="B9" s="129"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="129"/>
-      <c r="E9" s="129"/>
-      <c r="F9" s="129"/>
-      <c r="G9" s="129"/>
-      <c r="H9" s="129"/>
-      <c r="I9" s="129"/>
-      <c r="J9" s="129"/>
-      <c r="K9" s="129"/>
-      <c r="L9" s="129"/>
-      <c r="M9" s="129"/>
-      <c r="N9" s="129"/>
-      <c r="O9" s="129"/>
-      <c r="P9" s="129"/>
-      <c r="Q9" s="129"/>
-      <c r="R9" s="129"/>
-      <c r="S9" s="129"/>
-      <c r="T9" s="129"/>
-      <c r="U9" s="129"/>
-      <c r="V9" s="129"/>
-      <c r="W9" s="129"/>
-      <c r="X9" s="129"/>
-      <c r="Y9" s="129"/>
-      <c r="Z9" s="130"/>
+      <c r="A9" s="193"/>
+      <c r="B9" s="194"/>
+      <c r="C9" s="194"/>
+      <c r="D9" s="194"/>
+      <c r="E9" s="194"/>
+      <c r="F9" s="194"/>
+      <c r="G9" s="194"/>
+      <c r="H9" s="194"/>
+      <c r="I9" s="194"/>
+      <c r="J9" s="194"/>
+      <c r="K9" s="194"/>
+      <c r="L9" s="194"/>
+      <c r="M9" s="194"/>
+      <c r="N9" s="194"/>
+      <c r="O9" s="194"/>
+      <c r="P9" s="194"/>
+      <c r="Q9" s="194"/>
+      <c r="R9" s="194"/>
+      <c r="S9" s="194"/>
+      <c r="T9" s="194"/>
+      <c r="U9" s="194"/>
+      <c r="V9" s="194"/>
+      <c r="W9" s="194"/>
+      <c r="X9" s="194"/>
+      <c r="Y9" s="194"/>
+      <c r="Z9" s="195"/>
       <c r="AA9" s="69"/>
       <c r="AB9" s="54"/>
       <c r="AC9" s="54"/>
@@ -3179,21 +3143,21 @@
       <c r="AL9" s="54"/>
       <c r="AM9" s="54"/>
       <c r="AN9" s="54"/>
-      <c r="AO9" s="192"/>
-      <c r="AP9" s="193"/>
-      <c r="AQ9" s="193"/>
-      <c r="AR9" s="193"/>
-      <c r="AS9" s="193"/>
-      <c r="AT9" s="193"/>
-      <c r="AU9" s="193"/>
-      <c r="AV9" s="193"/>
-      <c r="AW9" s="193"/>
-      <c r="AX9" s="193"/>
-      <c r="AY9" s="193"/>
-      <c r="AZ9" s="193"/>
-      <c r="BA9" s="193"/>
-      <c r="BB9" s="193"/>
-      <c r="BC9" s="194"/>
+      <c r="AO9" s="99"/>
+      <c r="AP9" s="100"/>
+      <c r="AQ9" s="100"/>
+      <c r="AR9" s="100"/>
+      <c r="AS9" s="100"/>
+      <c r="AT9" s="100"/>
+      <c r="AU9" s="100"/>
+      <c r="AV9" s="100"/>
+      <c r="AW9" s="100"/>
+      <c r="AX9" s="100"/>
+      <c r="AY9" s="100"/>
+      <c r="AZ9" s="100"/>
+      <c r="BA9" s="100"/>
+      <c r="BB9" s="100"/>
+      <c r="BC9" s="101"/>
     </row>
     <row r="10" spans="1:55">
       <c r="A10" s="68" t="s">
@@ -3296,48 +3260,48 @@
       </c>
       <c r="R11" s="60"/>
       <c r="S11" s="59"/>
-      <c r="T11" s="195" t="s">
-        <v>61</v>
-      </c>
-      <c r="U11" s="196"/>
-      <c r="V11" s="196"/>
-      <c r="W11" s="196"/>
-      <c r="X11" s="196"/>
-      <c r="Y11" s="196"/>
-      <c r="Z11" s="196"/>
-      <c r="AA11" s="196"/>
-      <c r="AB11" s="196"/>
-      <c r="AC11" s="196"/>
-      <c r="AD11" s="196"/>
-      <c r="AE11" s="196"/>
-      <c r="AF11" s="196"/>
-      <c r="AG11" s="197"/>
-      <c r="AH11" s="204" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI11" s="205"/>
-      <c r="AJ11" s="205"/>
-      <c r="AK11" s="205"/>
-      <c r="AL11" s="205"/>
-      <c r="AM11" s="205"/>
-      <c r="AN11" s="205"/>
-      <c r="AO11" s="205"/>
-      <c r="AP11" s="206"/>
-      <c r="AQ11" s="213"/>
-      <c r="AR11" s="213"/>
-      <c r="AS11" s="213"/>
-      <c r="AT11" s="213"/>
-      <c r="AU11" s="213"/>
-      <c r="AV11" s="213"/>
-      <c r="AW11" s="213"/>
-      <c r="AX11" s="215" t="s">
-        <v>63</v>
-      </c>
-      <c r="AY11" s="215"/>
-      <c r="AZ11" s="215"/>
-      <c r="BA11" s="215"/>
-      <c r="BB11" s="216"/>
-      <c r="BC11" s="217"/>
+      <c r="T11" s="102" t="s">
+        <v>61</v>
+      </c>
+      <c r="U11" s="103"/>
+      <c r="V11" s="103"/>
+      <c r="W11" s="103"/>
+      <c r="X11" s="103"/>
+      <c r="Y11" s="103"/>
+      <c r="Z11" s="103"/>
+      <c r="AA11" s="103"/>
+      <c r="AB11" s="103"/>
+      <c r="AC11" s="103"/>
+      <c r="AD11" s="103"/>
+      <c r="AE11" s="103"/>
+      <c r="AF11" s="103"/>
+      <c r="AG11" s="104"/>
+      <c r="AH11" s="111" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI11" s="112"/>
+      <c r="AJ11" s="112"/>
+      <c r="AK11" s="112"/>
+      <c r="AL11" s="112"/>
+      <c r="AM11" s="112"/>
+      <c r="AN11" s="112"/>
+      <c r="AO11" s="112"/>
+      <c r="AP11" s="113"/>
+      <c r="AQ11" s="120"/>
+      <c r="AR11" s="120"/>
+      <c r="AS11" s="120"/>
+      <c r="AT11" s="120"/>
+      <c r="AU11" s="120"/>
+      <c r="AV11" s="120"/>
+      <c r="AW11" s="120"/>
+      <c r="AX11" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="AY11" s="122"/>
+      <c r="AZ11" s="122"/>
+      <c r="BA11" s="122"/>
+      <c r="BB11" s="123"/>
+      <c r="BC11" s="124"/>
     </row>
     <row r="12" spans="1:55">
       <c r="A12" s="58"/>
@@ -3369,42 +3333,42 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="56"/>
-      <c r="T12" s="198"/>
-      <c r="U12" s="199"/>
-      <c r="V12" s="199"/>
-      <c r="W12" s="199"/>
-      <c r="X12" s="199"/>
-      <c r="Y12" s="199"/>
-      <c r="Z12" s="199"/>
-      <c r="AA12" s="199"/>
-      <c r="AB12" s="199"/>
-      <c r="AC12" s="199"/>
-      <c r="AD12" s="199"/>
-      <c r="AE12" s="199"/>
-      <c r="AF12" s="199"/>
-      <c r="AG12" s="200"/>
-      <c r="AH12" s="207"/>
-      <c r="AI12" s="208"/>
-      <c r="AJ12" s="208"/>
-      <c r="AK12" s="208"/>
-      <c r="AL12" s="208"/>
-      <c r="AM12" s="208"/>
-      <c r="AN12" s="208"/>
-      <c r="AO12" s="208"/>
-      <c r="AP12" s="209"/>
-      <c r="AQ12" s="213"/>
-      <c r="AR12" s="213"/>
-      <c r="AS12" s="213"/>
-      <c r="AT12" s="213"/>
-      <c r="AU12" s="213"/>
-      <c r="AV12" s="213"/>
-      <c r="AW12" s="213"/>
-      <c r="AX12" s="215"/>
-      <c r="AY12" s="215"/>
-      <c r="AZ12" s="215"/>
-      <c r="BA12" s="215"/>
-      <c r="BB12" s="216"/>
-      <c r="BC12" s="217"/>
+      <c r="T12" s="105"/>
+      <c r="U12" s="106"/>
+      <c r="V12" s="106"/>
+      <c r="W12" s="106"/>
+      <c r="X12" s="106"/>
+      <c r="Y12" s="106"/>
+      <c r="Z12" s="106"/>
+      <c r="AA12" s="106"/>
+      <c r="AB12" s="106"/>
+      <c r="AC12" s="106"/>
+      <c r="AD12" s="106"/>
+      <c r="AE12" s="106"/>
+      <c r="AF12" s="106"/>
+      <c r="AG12" s="107"/>
+      <c r="AH12" s="114"/>
+      <c r="AI12" s="115"/>
+      <c r="AJ12" s="115"/>
+      <c r="AK12" s="115"/>
+      <c r="AL12" s="115"/>
+      <c r="AM12" s="115"/>
+      <c r="AN12" s="115"/>
+      <c r="AO12" s="115"/>
+      <c r="AP12" s="116"/>
+      <c r="AQ12" s="120"/>
+      <c r="AR12" s="120"/>
+      <c r="AS12" s="120"/>
+      <c r="AT12" s="120"/>
+      <c r="AU12" s="120"/>
+      <c r="AV12" s="120"/>
+      <c r="AW12" s="120"/>
+      <c r="AX12" s="122"/>
+      <c r="AY12" s="122"/>
+      <c r="AZ12" s="122"/>
+      <c r="BA12" s="122"/>
+      <c r="BB12" s="123"/>
+      <c r="BC12" s="124"/>
     </row>
     <row r="13" spans="1:55" ht="14" thickBot="1">
       <c r="A13" s="55"/>
@@ -3438,48 +3402,48 @@
       </c>
       <c r="R13" s="52"/>
       <c r="S13" s="51"/>
-      <c r="T13" s="201"/>
-      <c r="U13" s="202"/>
-      <c r="V13" s="202"/>
-      <c r="W13" s="202"/>
-      <c r="X13" s="202"/>
-      <c r="Y13" s="202"/>
-      <c r="Z13" s="202"/>
-      <c r="AA13" s="202"/>
-      <c r="AB13" s="202"/>
-      <c r="AC13" s="202"/>
-      <c r="AD13" s="202"/>
-      <c r="AE13" s="202"/>
-      <c r="AF13" s="202"/>
-      <c r="AG13" s="203"/>
-      <c r="AH13" s="210"/>
-      <c r="AI13" s="211"/>
-      <c r="AJ13" s="211"/>
-      <c r="AK13" s="211"/>
-      <c r="AL13" s="211"/>
-      <c r="AM13" s="211"/>
-      <c r="AN13" s="211"/>
-      <c r="AO13" s="211"/>
-      <c r="AP13" s="212"/>
-      <c r="AQ13" s="214"/>
-      <c r="AR13" s="214"/>
-      <c r="AS13" s="214"/>
-      <c r="AT13" s="214"/>
-      <c r="AU13" s="214"/>
-      <c r="AV13" s="214"/>
-      <c r="AW13" s="214"/>
-      <c r="AX13" s="218"/>
-      <c r="AY13" s="218"/>
-      <c r="AZ13" s="218"/>
-      <c r="BA13" s="218"/>
-      <c r="BB13" s="219"/>
-      <c r="BC13" s="220"/>
+      <c r="T13" s="108"/>
+      <c r="U13" s="109"/>
+      <c r="V13" s="109"/>
+      <c r="W13" s="109"/>
+      <c r="X13" s="109"/>
+      <c r="Y13" s="109"/>
+      <c r="Z13" s="109"/>
+      <c r="AA13" s="109"/>
+      <c r="AB13" s="109"/>
+      <c r="AC13" s="109"/>
+      <c r="AD13" s="109"/>
+      <c r="AE13" s="109"/>
+      <c r="AF13" s="109"/>
+      <c r="AG13" s="110"/>
+      <c r="AH13" s="117"/>
+      <c r="AI13" s="118"/>
+      <c r="AJ13" s="118"/>
+      <c r="AK13" s="118"/>
+      <c r="AL13" s="118"/>
+      <c r="AM13" s="118"/>
+      <c r="AN13" s="118"/>
+      <c r="AO13" s="118"/>
+      <c r="AP13" s="119"/>
+      <c r="AQ13" s="121"/>
+      <c r="AR13" s="121"/>
+      <c r="AS13" s="121"/>
+      <c r="AT13" s="121"/>
+      <c r="AU13" s="121"/>
+      <c r="AV13" s="121"/>
+      <c r="AW13" s="121"/>
+      <c r="AX13" s="125"/>
+      <c r="AY13" s="125"/>
+      <c r="AZ13" s="125"/>
+      <c r="BA13" s="125"/>
+      <c r="BB13" s="126"/>
+      <c r="BC13" s="127"/>
     </row>
     <row r="14" spans="1:55">
-      <c r="A14" s="141" t="s">
+      <c r="A14" s="200" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="142"/>
+      <c r="B14" s="201"/>
       <c r="C14" s="48" t="s">
         <v>17</v>
       </c>
@@ -3547,10 +3511,10 @@
       <c r="BC14" s="46"/>
     </row>
     <row r="15" spans="1:55">
-      <c r="A15" s="122" t="s">
+      <c r="A15" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="123"/>
+      <c r="B15" s="130"/>
       <c r="C15" s="35" t="s">
         <v>24</v>
       </c>
@@ -3570,10 +3534,10 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
-      <c r="T15" s="124" t="s">
+      <c r="T15" s="208" t="s">
         <v>45</v>
       </c>
-      <c r="U15" s="123"/>
+      <c r="U15" s="130"/>
       <c r="V15" s="39" t="s">
         <v>25</v>
       </c>
@@ -3601,8 +3565,8 @@
       <c r="BC15" s="34"/>
     </row>
     <row r="16" spans="1:55">
-      <c r="A16" s="122"/>
-      <c r="B16" s="123"/>
+      <c r="A16" s="128"/>
+      <c r="B16" s="130"/>
       <c r="C16" s="35"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -3620,10 +3584,10 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
-      <c r="T16" s="124" t="s">
+      <c r="T16" s="208" t="s">
         <v>44</v>
       </c>
-      <c r="U16" s="123"/>
+      <c r="U16" s="130"/>
       <c r="V16" s="39" t="s">
         <v>29</v>
       </c>
@@ -3655,8 +3619,8 @@
       <c r="BC16" s="40"/>
     </row>
     <row r="17" spans="1:56">
-      <c r="A17" s="122"/>
-      <c r="B17" s="123"/>
+      <c r="A17" s="128"/>
+      <c r="B17" s="130"/>
       <c r="C17" s="35"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -3674,10 +3638,10 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
-      <c r="T17" s="184" t="s">
+      <c r="T17" s="153" t="s">
         <v>42</v>
       </c>
-      <c r="U17" s="185"/>
+      <c r="U17" s="154"/>
       <c r="V17" s="39" t="s">
         <v>32</v>
       </c>
@@ -3703,43 +3667,43 @@
       <c r="BC17" s="34"/>
     </row>
     <row r="18" spans="1:56">
-      <c r="A18" s="183">
+      <c r="A18" s="149">
         <v>1</v>
       </c>
-      <c r="B18" s="171"/>
-      <c r="C18" s="104">
+      <c r="B18" s="150"/>
+      <c r="C18" s="151">
         <v>2</v>
       </c>
-      <c r="D18" s="105"/>
-      <c r="E18" s="105"/>
-      <c r="F18" s="105"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="105"/>
-      <c r="I18" s="105"/>
-      <c r="J18" s="105"/>
-      <c r="K18" s="105"/>
-      <c r="L18" s="105"/>
-      <c r="M18" s="105"/>
-      <c r="N18" s="105"/>
-      <c r="O18" s="105"/>
-      <c r="P18" s="105"/>
-      <c r="Q18" s="105"/>
-      <c r="R18" s="105"/>
-      <c r="S18" s="171"/>
-      <c r="T18" s="104">
+      <c r="D18" s="152"/>
+      <c r="E18" s="152"/>
+      <c r="F18" s="152"/>
+      <c r="G18" s="152"/>
+      <c r="H18" s="152"/>
+      <c r="I18" s="152"/>
+      <c r="J18" s="152"/>
+      <c r="K18" s="152"/>
+      <c r="L18" s="152"/>
+      <c r="M18" s="152"/>
+      <c r="N18" s="152"/>
+      <c r="O18" s="152"/>
+      <c r="P18" s="152"/>
+      <c r="Q18" s="152"/>
+      <c r="R18" s="152"/>
+      <c r="S18" s="150"/>
+      <c r="T18" s="151">
         <v>3</v>
       </c>
-      <c r="U18" s="171"/>
-      <c r="V18" s="104">
+      <c r="U18" s="150"/>
+      <c r="V18" s="151">
         <v>4</v>
       </c>
-      <c r="W18" s="105"/>
-      <c r="X18" s="105"/>
-      <c r="Y18" s="171"/>
-      <c r="Z18" s="104">
+      <c r="W18" s="152"/>
+      <c r="X18" s="152"/>
+      <c r="Y18" s="150"/>
+      <c r="Z18" s="151">
         <v>5</v>
       </c>
-      <c r="AA18" s="171"/>
+      <c r="AA18" s="150"/>
       <c r="AB18" s="33" t="s">
         <v>35</v>
       </c>
@@ -3760,81 +3724,81 @@
       <c r="AO18" s="30"/>
       <c r="AP18" s="30"/>
       <c r="AQ18" s="29"/>
-      <c r="AR18" s="104">
+      <c r="AR18" s="151">
         <v>7</v>
       </c>
-      <c r="AS18" s="105"/>
-      <c r="AT18" s="105"/>
-      <c r="AU18" s="105"/>
-      <c r="AV18" s="105"/>
-      <c r="AW18" s="105"/>
-      <c r="AX18" s="105"/>
-      <c r="AY18" s="105"/>
-      <c r="AZ18" s="171"/>
-      <c r="BA18" s="104">
+      <c r="AS18" s="152"/>
+      <c r="AT18" s="152"/>
+      <c r="AU18" s="152"/>
+      <c r="AV18" s="152"/>
+      <c r="AW18" s="152"/>
+      <c r="AX18" s="152"/>
+      <c r="AY18" s="152"/>
+      <c r="AZ18" s="150"/>
+      <c r="BA18" s="151">
         <v>8</v>
       </c>
-      <c r="BB18" s="105"/>
-      <c r="BC18" s="106"/>
+      <c r="BB18" s="152"/>
+      <c r="BC18" s="216"/>
     </row>
     <row r="19" spans="1:56" ht="24.5" customHeight="1">
-      <c r="A19" s="137">
+      <c r="A19" s="196">
         <v>1</v>
       </c>
-      <c r="B19" s="138"/>
-      <c r="C19" s="180" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="181"/>
-      <c r="E19" s="181"/>
-      <c r="F19" s="181"/>
-      <c r="G19" s="181"/>
-      <c r="H19" s="181"/>
-      <c r="I19" s="181"/>
-      <c r="J19" s="181"/>
-      <c r="K19" s="181"/>
-      <c r="L19" s="181"/>
-      <c r="M19" s="181"/>
-      <c r="N19" s="181"/>
-      <c r="O19" s="181"/>
-      <c r="P19" s="181"/>
-      <c r="Q19" s="181"/>
-      <c r="R19" s="181"/>
-      <c r="S19" s="182"/>
-      <c r="T19" s="112" t="s">
-        <v>61</v>
-      </c>
-      <c r="U19" s="113"/>
-      <c r="V19" s="172" t="s">
-        <v>61</v>
-      </c>
-      <c r="W19" s="173"/>
-      <c r="X19" s="173"/>
-      <c r="Y19" s="174"/>
-      <c r="Z19" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA19" s="103"/>
-      <c r="AB19" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC19" s="121"/>
-      <c r="AD19" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE19" s="95"/>
-      <c r="AF19" s="95"/>
-      <c r="AG19" s="95"/>
-      <c r="AH19" s="95"/>
-      <c r="AI19" s="95"/>
-      <c r="AJ19" s="95"/>
-      <c r="AK19" s="95"/>
-      <c r="AL19" s="95"/>
-      <c r="AM19" s="95"/>
-      <c r="AN19" s="95"/>
-      <c r="AO19" s="95"/>
-      <c r="AP19" s="95"/>
-      <c r="AQ19" s="96"/>
+      <c r="B19" s="197"/>
+      <c r="C19" s="143" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="144"/>
+      <c r="E19" s="144"/>
+      <c r="F19" s="144"/>
+      <c r="G19" s="144"/>
+      <c r="H19" s="144"/>
+      <c r="I19" s="144"/>
+      <c r="J19" s="144"/>
+      <c r="K19" s="144"/>
+      <c r="L19" s="144"/>
+      <c r="M19" s="144"/>
+      <c r="N19" s="144"/>
+      <c r="O19" s="144"/>
+      <c r="P19" s="144"/>
+      <c r="Q19" s="144"/>
+      <c r="R19" s="144"/>
+      <c r="S19" s="145"/>
+      <c r="T19" s="189" t="s">
+        <v>61</v>
+      </c>
+      <c r="U19" s="190"/>
+      <c r="V19" s="202" t="s">
+        <v>61</v>
+      </c>
+      <c r="W19" s="203"/>
+      <c r="X19" s="203"/>
+      <c r="Y19" s="204"/>
+      <c r="Z19" s="141" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA19" s="137"/>
+      <c r="AB19" s="141" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC19" s="142"/>
+      <c r="AD19" s="209" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE19" s="210"/>
+      <c r="AF19" s="210"/>
+      <c r="AG19" s="210"/>
+      <c r="AH19" s="210"/>
+      <c r="AI19" s="210"/>
+      <c r="AJ19" s="210"/>
+      <c r="AK19" s="210"/>
+      <c r="AL19" s="210"/>
+      <c r="AM19" s="210"/>
+      <c r="AN19" s="210"/>
+      <c r="AO19" s="210"/>
+      <c r="AP19" s="210"/>
+      <c r="AQ19" s="211"/>
       <c r="AR19" s="28"/>
       <c r="AS19" s="27"/>
       <c r="AT19" s="27"/>
@@ -3844,73 +3808,73 @@
       <c r="AX19" s="27"/>
       <c r="AY19" s="26"/>
       <c r="AZ19" s="26"/>
-      <c r="BA19" s="107" t="s">
-        <v>61</v>
-      </c>
-      <c r="BB19" s="108"/>
-      <c r="BC19" s="109"/>
+      <c r="BA19" s="217" t="s">
+        <v>61</v>
+      </c>
+      <c r="BB19" s="218"/>
+      <c r="BC19" s="219"/>
       <c r="BD19" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:56" ht="24.5" customHeight="1">
-      <c r="A20" s="139" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="140"/>
-      <c r="C20" s="134" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="135"/>
-      <c r="E20" s="135"/>
-      <c r="F20" s="135"/>
-      <c r="G20" s="135"/>
-      <c r="H20" s="135"/>
-      <c r="I20" s="135"/>
-      <c r="J20" s="135"/>
-      <c r="K20" s="135"/>
-      <c r="L20" s="135"/>
-      <c r="M20" s="135"/>
-      <c r="N20" s="135"/>
-      <c r="O20" s="135"/>
-      <c r="P20" s="135"/>
-      <c r="Q20" s="135"/>
-      <c r="R20" s="135"/>
-      <c r="S20" s="136"/>
-      <c r="T20" s="110" t="s">
-        <v>61</v>
-      </c>
-      <c r="U20" s="111"/>
-      <c r="V20" s="222" t="s">
-        <v>61</v>
-      </c>
-      <c r="W20" s="223"/>
-      <c r="X20" s="223"/>
-      <c r="Y20" s="224"/>
-      <c r="Z20" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA20" s="101"/>
-      <c r="AB20" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC20" s="120"/>
-      <c r="AD20" s="97" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE20" s="98"/>
-      <c r="AF20" s="98"/>
-      <c r="AG20" s="98"/>
-      <c r="AH20" s="98"/>
-      <c r="AI20" s="98"/>
-      <c r="AJ20" s="98"/>
-      <c r="AK20" s="98"/>
-      <c r="AL20" s="98"/>
-      <c r="AM20" s="98"/>
-      <c r="AN20" s="98"/>
-      <c r="AO20" s="98"/>
-      <c r="AP20" s="98"/>
-      <c r="AQ20" s="99"/>
+      <c r="A20" s="198" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="199"/>
+      <c r="C20" s="146" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="147"/>
+      <c r="E20" s="147"/>
+      <c r="F20" s="147"/>
+      <c r="G20" s="147"/>
+      <c r="H20" s="147"/>
+      <c r="I20" s="147"/>
+      <c r="J20" s="147"/>
+      <c r="K20" s="147"/>
+      <c r="L20" s="147"/>
+      <c r="M20" s="147"/>
+      <c r="N20" s="147"/>
+      <c r="O20" s="147"/>
+      <c r="P20" s="147"/>
+      <c r="Q20" s="147"/>
+      <c r="R20" s="147"/>
+      <c r="S20" s="148"/>
+      <c r="T20" s="191" t="s">
+        <v>61</v>
+      </c>
+      <c r="U20" s="192"/>
+      <c r="V20" s="205" t="s">
+        <v>61</v>
+      </c>
+      <c r="W20" s="206"/>
+      <c r="X20" s="206"/>
+      <c r="Y20" s="207"/>
+      <c r="Z20" s="184" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA20" s="212"/>
+      <c r="AB20" s="184" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC20" s="185"/>
+      <c r="AD20" s="213" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE20" s="214"/>
+      <c r="AF20" s="214"/>
+      <c r="AG20" s="214"/>
+      <c r="AH20" s="214"/>
+      <c r="AI20" s="214"/>
+      <c r="AJ20" s="214"/>
+      <c r="AK20" s="214"/>
+      <c r="AL20" s="214"/>
+      <c r="AM20" s="214"/>
+      <c r="AN20" s="214"/>
+      <c r="AO20" s="214"/>
+      <c r="AP20" s="214"/>
+      <c r="AQ20" s="215"/>
       <c r="AR20" s="25"/>
       <c r="AS20" s="24"/>
       <c r="AT20" s="24"/>
@@ -3920,73 +3884,73 @@
       <c r="AX20" s="24"/>
       <c r="AY20" s="23"/>
       <c r="AZ20" s="23"/>
-      <c r="BA20" s="175" t="s">
-        <v>61</v>
-      </c>
-      <c r="BB20" s="176"/>
-      <c r="BC20" s="177"/>
+      <c r="BA20" s="220" t="s">
+        <v>61</v>
+      </c>
+      <c r="BB20" s="221"/>
+      <c r="BC20" s="222"/>
       <c r="BD20" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:56" ht="24.5" customHeight="1">
-      <c r="A21" s="133" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="103"/>
-      <c r="C21" s="143" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="144"/>
-      <c r="E21" s="144"/>
-      <c r="F21" s="144"/>
-      <c r="G21" s="144"/>
-      <c r="H21" s="144"/>
-      <c r="I21" s="144"/>
-      <c r="J21" s="144"/>
-      <c r="K21" s="144"/>
-      <c r="L21" s="144"/>
-      <c r="M21" s="144"/>
-      <c r="N21" s="144"/>
-      <c r="O21" s="144"/>
-      <c r="P21" s="144"/>
-      <c r="Q21" s="144"/>
-      <c r="R21" s="144"/>
-      <c r="S21" s="145"/>
-      <c r="T21" s="112" t="s">
-        <v>61</v>
-      </c>
-      <c r="U21" s="113"/>
-      <c r="V21" s="172" t="s">
-        <v>61</v>
-      </c>
-      <c r="W21" s="173"/>
-      <c r="X21" s="173"/>
-      <c r="Y21" s="174"/>
-      <c r="Z21" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA21" s="103"/>
-      <c r="AB21" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC21" s="121"/>
-      <c r="AD21" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE21" s="95"/>
-      <c r="AF21" s="95"/>
-      <c r="AG21" s="95"/>
-      <c r="AH21" s="95"/>
-      <c r="AI21" s="95"/>
-      <c r="AJ21" s="95"/>
-      <c r="AK21" s="95"/>
-      <c r="AL21" s="95"/>
-      <c r="AM21" s="95"/>
-      <c r="AN21" s="95"/>
-      <c r="AO21" s="95"/>
-      <c r="AP21" s="95"/>
-      <c r="AQ21" s="96"/>
+      <c r="A21" s="136" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="137"/>
+      <c r="C21" s="186" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="187"/>
+      <c r="E21" s="187"/>
+      <c r="F21" s="187"/>
+      <c r="G21" s="187"/>
+      <c r="H21" s="187"/>
+      <c r="I21" s="187"/>
+      <c r="J21" s="187"/>
+      <c r="K21" s="187"/>
+      <c r="L21" s="187"/>
+      <c r="M21" s="187"/>
+      <c r="N21" s="187"/>
+      <c r="O21" s="187"/>
+      <c r="P21" s="187"/>
+      <c r="Q21" s="187"/>
+      <c r="R21" s="187"/>
+      <c r="S21" s="188"/>
+      <c r="T21" s="189" t="s">
+        <v>61</v>
+      </c>
+      <c r="U21" s="190"/>
+      <c r="V21" s="202" t="s">
+        <v>61</v>
+      </c>
+      <c r="W21" s="203"/>
+      <c r="X21" s="203"/>
+      <c r="Y21" s="204"/>
+      <c r="Z21" s="141" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA21" s="137"/>
+      <c r="AB21" s="141" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC21" s="142"/>
+      <c r="AD21" s="209" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE21" s="210"/>
+      <c r="AF21" s="210"/>
+      <c r="AG21" s="210"/>
+      <c r="AH21" s="210"/>
+      <c r="AI21" s="210"/>
+      <c r="AJ21" s="210"/>
+      <c r="AK21" s="210"/>
+      <c r="AL21" s="210"/>
+      <c r="AM21" s="210"/>
+      <c r="AN21" s="210"/>
+      <c r="AO21" s="210"/>
+      <c r="AP21" s="210"/>
+      <c r="AQ21" s="211"/>
       <c r="AR21" s="19"/>
       <c r="AS21" s="18"/>
       <c r="AT21" s="18"/>
@@ -3996,73 +3960,73 @@
       <c r="AX21" s="18"/>
       <c r="AY21" s="17"/>
       <c r="AZ21" s="17"/>
-      <c r="BA21" s="117" t="s">
-        <v>61</v>
-      </c>
-      <c r="BB21" s="118"/>
-      <c r="BC21" s="119"/>
+      <c r="BA21" s="138" t="s">
+        <v>61</v>
+      </c>
+      <c r="BB21" s="139"/>
+      <c r="BC21" s="140"/>
       <c r="BD21" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:56" ht="24.5" customHeight="1">
-      <c r="A22" s="131" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="132"/>
-      <c r="C22" s="134" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="135"/>
-      <c r="E22" s="135"/>
-      <c r="F22" s="135"/>
-      <c r="G22" s="135"/>
-      <c r="H22" s="135"/>
-      <c r="I22" s="135"/>
-      <c r="J22" s="135"/>
-      <c r="K22" s="135"/>
-      <c r="L22" s="135"/>
-      <c r="M22" s="135"/>
-      <c r="N22" s="135"/>
-      <c r="O22" s="135"/>
-      <c r="P22" s="135"/>
-      <c r="Q22" s="135"/>
-      <c r="R22" s="135"/>
-      <c r="S22" s="136"/>
-      <c r="T22" s="110" t="s">
-        <v>61</v>
-      </c>
-      <c r="U22" s="111"/>
-      <c r="V22" s="222" t="s">
-        <v>61</v>
-      </c>
-      <c r="W22" s="223"/>
-      <c r="X22" s="223"/>
-      <c r="Y22" s="224"/>
-      <c r="Z22" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA22" s="101"/>
-      <c r="AB22" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC22" s="120"/>
-      <c r="AD22" s="97" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE22" s="98"/>
-      <c r="AF22" s="98"/>
-      <c r="AG22" s="98"/>
-      <c r="AH22" s="98"/>
-      <c r="AI22" s="98"/>
-      <c r="AJ22" s="98"/>
-      <c r="AK22" s="98"/>
-      <c r="AL22" s="98"/>
-      <c r="AM22" s="98"/>
-      <c r="AN22" s="98"/>
-      <c r="AO22" s="98"/>
-      <c r="AP22" s="98"/>
-      <c r="AQ22" s="99"/>
+      <c r="A22" s="165" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="166"/>
+      <c r="C22" s="146" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="147"/>
+      <c r="E22" s="147"/>
+      <c r="F22" s="147"/>
+      <c r="G22" s="147"/>
+      <c r="H22" s="147"/>
+      <c r="I22" s="147"/>
+      <c r="J22" s="147"/>
+      <c r="K22" s="147"/>
+      <c r="L22" s="147"/>
+      <c r="M22" s="147"/>
+      <c r="N22" s="147"/>
+      <c r="O22" s="147"/>
+      <c r="P22" s="147"/>
+      <c r="Q22" s="147"/>
+      <c r="R22" s="147"/>
+      <c r="S22" s="148"/>
+      <c r="T22" s="191" t="s">
+        <v>61</v>
+      </c>
+      <c r="U22" s="192"/>
+      <c r="V22" s="205" t="s">
+        <v>61</v>
+      </c>
+      <c r="W22" s="206"/>
+      <c r="X22" s="206"/>
+      <c r="Y22" s="207"/>
+      <c r="Z22" s="184" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA22" s="212"/>
+      <c r="AB22" s="184" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC22" s="185"/>
+      <c r="AD22" s="213" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE22" s="214"/>
+      <c r="AF22" s="214"/>
+      <c r="AG22" s="214"/>
+      <c r="AH22" s="214"/>
+      <c r="AI22" s="214"/>
+      <c r="AJ22" s="214"/>
+      <c r="AK22" s="214"/>
+      <c r="AL22" s="214"/>
+      <c r="AM22" s="214"/>
+      <c r="AN22" s="214"/>
+      <c r="AO22" s="214"/>
+      <c r="AP22" s="214"/>
+      <c r="AQ22" s="215"/>
       <c r="AR22" s="22"/>
       <c r="AS22" s="21"/>
       <c r="AT22" s="21"/>
@@ -4072,73 +4036,73 @@
       <c r="AX22" s="21"/>
       <c r="AY22" s="20"/>
       <c r="AZ22" s="20"/>
-      <c r="BA22" s="114" t="s">
-        <v>61</v>
-      </c>
-      <c r="BB22" s="115"/>
-      <c r="BC22" s="116"/>
+      <c r="BA22" s="167" t="s">
+        <v>61</v>
+      </c>
+      <c r="BB22" s="168"/>
+      <c r="BC22" s="169"/>
       <c r="BD22" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:56" ht="24.5" customHeight="1">
-      <c r="A23" s="133" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="103"/>
-      <c r="C23" s="143" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="144"/>
-      <c r="H23" s="144"/>
-      <c r="I23" s="144"/>
-      <c r="J23" s="144"/>
-      <c r="K23" s="144"/>
-      <c r="L23" s="144"/>
-      <c r="M23" s="144"/>
-      <c r="N23" s="144"/>
-      <c r="O23" s="144"/>
-      <c r="P23" s="144"/>
-      <c r="Q23" s="144"/>
-      <c r="R23" s="144"/>
-      <c r="S23" s="145"/>
-      <c r="T23" s="112" t="s">
-        <v>61</v>
-      </c>
-      <c r="U23" s="113"/>
-      <c r="V23" s="172" t="s">
-        <v>61</v>
-      </c>
-      <c r="W23" s="173"/>
-      <c r="X23" s="173"/>
-      <c r="Y23" s="174"/>
-      <c r="Z23" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA23" s="103"/>
-      <c r="AB23" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC23" s="121"/>
-      <c r="AD23" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE23" s="95"/>
-      <c r="AF23" s="95"/>
-      <c r="AG23" s="95"/>
-      <c r="AH23" s="95"/>
-      <c r="AI23" s="95"/>
-      <c r="AJ23" s="95"/>
-      <c r="AK23" s="95"/>
-      <c r="AL23" s="95"/>
-      <c r="AM23" s="95"/>
-      <c r="AN23" s="95"/>
-      <c r="AO23" s="95"/>
-      <c r="AP23" s="95"/>
-      <c r="AQ23" s="96"/>
+      <c r="A23" s="136" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="137"/>
+      <c r="C23" s="186" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="187"/>
+      <c r="E23" s="187"/>
+      <c r="F23" s="187"/>
+      <c r="G23" s="187"/>
+      <c r="H23" s="187"/>
+      <c r="I23" s="187"/>
+      <c r="J23" s="187"/>
+      <c r="K23" s="187"/>
+      <c r="L23" s="187"/>
+      <c r="M23" s="187"/>
+      <c r="N23" s="187"/>
+      <c r="O23" s="187"/>
+      <c r="P23" s="187"/>
+      <c r="Q23" s="187"/>
+      <c r="R23" s="187"/>
+      <c r="S23" s="188"/>
+      <c r="T23" s="189" t="s">
+        <v>61</v>
+      </c>
+      <c r="U23" s="190"/>
+      <c r="V23" s="202" t="s">
+        <v>61</v>
+      </c>
+      <c r="W23" s="203"/>
+      <c r="X23" s="203"/>
+      <c r="Y23" s="204"/>
+      <c r="Z23" s="141" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA23" s="137"/>
+      <c r="AB23" s="141" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC23" s="142"/>
+      <c r="AD23" s="209" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE23" s="210"/>
+      <c r="AF23" s="210"/>
+      <c r="AG23" s="210"/>
+      <c r="AH23" s="210"/>
+      <c r="AI23" s="210"/>
+      <c r="AJ23" s="210"/>
+      <c r="AK23" s="210"/>
+      <c r="AL23" s="210"/>
+      <c r="AM23" s="210"/>
+      <c r="AN23" s="210"/>
+      <c r="AO23" s="210"/>
+      <c r="AP23" s="210"/>
+      <c r="AQ23" s="211"/>
       <c r="AR23" s="19"/>
       <c r="AS23" s="18"/>
       <c r="AT23" s="18"/>
@@ -4148,73 +4112,73 @@
       <c r="AX23" s="18"/>
       <c r="AY23" s="17"/>
       <c r="AZ23" s="17"/>
-      <c r="BA23" s="117" t="s">
-        <v>61</v>
-      </c>
-      <c r="BB23" s="118"/>
-      <c r="BC23" s="119"/>
+      <c r="BA23" s="138" t="s">
+        <v>61</v>
+      </c>
+      <c r="BB23" s="139"/>
+      <c r="BC23" s="140"/>
       <c r="BD23" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:56" ht="24.5" customHeight="1">
-      <c r="A24" s="131" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="132"/>
-      <c r="C24" s="134" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="135"/>
-      <c r="E24" s="135"/>
-      <c r="F24" s="135"/>
-      <c r="G24" s="135"/>
-      <c r="H24" s="135"/>
-      <c r="I24" s="135"/>
-      <c r="J24" s="135"/>
-      <c r="K24" s="135"/>
-      <c r="L24" s="135"/>
-      <c r="M24" s="135"/>
-      <c r="N24" s="135"/>
-      <c r="O24" s="135"/>
-      <c r="P24" s="135"/>
-      <c r="Q24" s="135"/>
-      <c r="R24" s="135"/>
-      <c r="S24" s="136"/>
-      <c r="T24" s="110" t="s">
-        <v>61</v>
-      </c>
-      <c r="U24" s="111"/>
-      <c r="V24" s="222" t="s">
-        <v>61</v>
-      </c>
-      <c r="W24" s="223"/>
-      <c r="X24" s="223"/>
-      <c r="Y24" s="224"/>
-      <c r="Z24" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA24" s="101"/>
-      <c r="AB24" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC24" s="120"/>
-      <c r="AD24" s="97" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE24" s="98"/>
-      <c r="AF24" s="98"/>
-      <c r="AG24" s="98"/>
-      <c r="AH24" s="98"/>
-      <c r="AI24" s="98"/>
-      <c r="AJ24" s="98"/>
-      <c r="AK24" s="98"/>
-      <c r="AL24" s="98"/>
-      <c r="AM24" s="98"/>
-      <c r="AN24" s="98"/>
-      <c r="AO24" s="98"/>
-      <c r="AP24" s="98"/>
-      <c r="AQ24" s="99"/>
+      <c r="A24" s="165" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="166"/>
+      <c r="C24" s="146" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="147"/>
+      <c r="E24" s="147"/>
+      <c r="F24" s="147"/>
+      <c r="G24" s="147"/>
+      <c r="H24" s="147"/>
+      <c r="I24" s="147"/>
+      <c r="J24" s="147"/>
+      <c r="K24" s="147"/>
+      <c r="L24" s="147"/>
+      <c r="M24" s="147"/>
+      <c r="N24" s="147"/>
+      <c r="O24" s="147"/>
+      <c r="P24" s="147"/>
+      <c r="Q24" s="147"/>
+      <c r="R24" s="147"/>
+      <c r="S24" s="148"/>
+      <c r="T24" s="191" t="s">
+        <v>61</v>
+      </c>
+      <c r="U24" s="192"/>
+      <c r="V24" s="205" t="s">
+        <v>61</v>
+      </c>
+      <c r="W24" s="206"/>
+      <c r="X24" s="206"/>
+      <c r="Y24" s="207"/>
+      <c r="Z24" s="184" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA24" s="212"/>
+      <c r="AB24" s="184" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC24" s="185"/>
+      <c r="AD24" s="213" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE24" s="214"/>
+      <c r="AF24" s="214"/>
+      <c r="AG24" s="214"/>
+      <c r="AH24" s="214"/>
+      <c r="AI24" s="214"/>
+      <c r="AJ24" s="214"/>
+      <c r="AK24" s="214"/>
+      <c r="AL24" s="214"/>
+      <c r="AM24" s="214"/>
+      <c r="AN24" s="214"/>
+      <c r="AO24" s="214"/>
+      <c r="AP24" s="214"/>
+      <c r="AQ24" s="215"/>
       <c r="AR24" s="22"/>
       <c r="AS24" s="21"/>
       <c r="AT24" s="21"/>
@@ -4224,73 +4188,73 @@
       <c r="AX24" s="21"/>
       <c r="AY24" s="20"/>
       <c r="AZ24" s="20"/>
-      <c r="BA24" s="114" t="s">
-        <v>61</v>
-      </c>
-      <c r="BB24" s="115"/>
-      <c r="BC24" s="116"/>
+      <c r="BA24" s="167" t="s">
+        <v>61</v>
+      </c>
+      <c r="BB24" s="168"/>
+      <c r="BC24" s="169"/>
       <c r="BD24" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:56" ht="24.5" customHeight="1">
-      <c r="A25" s="133" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="103"/>
-      <c r="C25" s="143" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="144"/>
-      <c r="E25" s="144"/>
-      <c r="F25" s="144"/>
-      <c r="G25" s="144"/>
-      <c r="H25" s="144"/>
-      <c r="I25" s="144"/>
-      <c r="J25" s="144"/>
-      <c r="K25" s="144"/>
-      <c r="L25" s="144"/>
-      <c r="M25" s="144"/>
-      <c r="N25" s="144"/>
-      <c r="O25" s="144"/>
-      <c r="P25" s="144"/>
-      <c r="Q25" s="144"/>
-      <c r="R25" s="144"/>
-      <c r="S25" s="145"/>
-      <c r="T25" s="112" t="s">
-        <v>61</v>
-      </c>
-      <c r="U25" s="113"/>
-      <c r="V25" s="172" t="s">
-        <v>61</v>
-      </c>
-      <c r="W25" s="173"/>
-      <c r="X25" s="173"/>
-      <c r="Y25" s="174"/>
-      <c r="Z25" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA25" s="103"/>
-      <c r="AB25" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC25" s="121"/>
-      <c r="AD25" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE25" s="95"/>
-      <c r="AF25" s="95"/>
-      <c r="AG25" s="95"/>
-      <c r="AH25" s="95"/>
-      <c r="AI25" s="95"/>
-      <c r="AJ25" s="95"/>
-      <c r="AK25" s="95"/>
-      <c r="AL25" s="95"/>
-      <c r="AM25" s="95"/>
-      <c r="AN25" s="95"/>
-      <c r="AO25" s="95"/>
-      <c r="AP25" s="95"/>
-      <c r="AQ25" s="96"/>
+      <c r="A25" s="136" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="137"/>
+      <c r="C25" s="186" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="187"/>
+      <c r="E25" s="187"/>
+      <c r="F25" s="187"/>
+      <c r="G25" s="187"/>
+      <c r="H25" s="187"/>
+      <c r="I25" s="187"/>
+      <c r="J25" s="187"/>
+      <c r="K25" s="187"/>
+      <c r="L25" s="187"/>
+      <c r="M25" s="187"/>
+      <c r="N25" s="187"/>
+      <c r="O25" s="187"/>
+      <c r="P25" s="187"/>
+      <c r="Q25" s="187"/>
+      <c r="R25" s="187"/>
+      <c r="S25" s="188"/>
+      <c r="T25" s="189" t="s">
+        <v>61</v>
+      </c>
+      <c r="U25" s="190"/>
+      <c r="V25" s="202" t="s">
+        <v>61</v>
+      </c>
+      <c r="W25" s="203"/>
+      <c r="X25" s="203"/>
+      <c r="Y25" s="204"/>
+      <c r="Z25" s="141" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA25" s="137"/>
+      <c r="AB25" s="141" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC25" s="142"/>
+      <c r="AD25" s="209" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE25" s="210"/>
+      <c r="AF25" s="210"/>
+      <c r="AG25" s="210"/>
+      <c r="AH25" s="210"/>
+      <c r="AI25" s="210"/>
+      <c r="AJ25" s="210"/>
+      <c r="AK25" s="210"/>
+      <c r="AL25" s="210"/>
+      <c r="AM25" s="210"/>
+      <c r="AN25" s="210"/>
+      <c r="AO25" s="210"/>
+      <c r="AP25" s="210"/>
+      <c r="AQ25" s="211"/>
       <c r="AR25" s="19"/>
       <c r="AS25" s="18"/>
       <c r="AT25" s="18"/>
@@ -4300,73 +4264,73 @@
       <c r="AX25" s="18"/>
       <c r="AY25" s="17"/>
       <c r="AZ25" s="17"/>
-      <c r="BA25" s="117" t="s">
-        <v>61</v>
-      </c>
-      <c r="BB25" s="118"/>
-      <c r="BC25" s="119"/>
+      <c r="BA25" s="138" t="s">
+        <v>61</v>
+      </c>
+      <c r="BB25" s="139"/>
+      <c r="BC25" s="140"/>
       <c r="BD25" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:56" ht="24.5" customHeight="1">
-      <c r="A26" s="131" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="132"/>
-      <c r="C26" s="134" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="135"/>
-      <c r="E26" s="135"/>
-      <c r="F26" s="135"/>
-      <c r="G26" s="135"/>
-      <c r="H26" s="135"/>
-      <c r="I26" s="135"/>
-      <c r="J26" s="135"/>
-      <c r="K26" s="135"/>
-      <c r="L26" s="135"/>
-      <c r="M26" s="135"/>
-      <c r="N26" s="135"/>
-      <c r="O26" s="135"/>
-      <c r="P26" s="135"/>
-      <c r="Q26" s="135"/>
-      <c r="R26" s="135"/>
-      <c r="S26" s="136"/>
-      <c r="T26" s="110" t="s">
-        <v>61</v>
-      </c>
-      <c r="U26" s="111"/>
-      <c r="V26" s="222" t="s">
-        <v>61</v>
-      </c>
-      <c r="W26" s="223"/>
-      <c r="X26" s="223"/>
-      <c r="Y26" s="224"/>
-      <c r="Z26" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA26" s="101"/>
-      <c r="AB26" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC26" s="120"/>
-      <c r="AD26" s="97" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE26" s="98"/>
-      <c r="AF26" s="98"/>
-      <c r="AG26" s="98"/>
-      <c r="AH26" s="98"/>
-      <c r="AI26" s="98"/>
-      <c r="AJ26" s="98"/>
-      <c r="AK26" s="98"/>
-      <c r="AL26" s="98"/>
-      <c r="AM26" s="98"/>
-      <c r="AN26" s="98"/>
-      <c r="AO26" s="98"/>
-      <c r="AP26" s="98"/>
-      <c r="AQ26" s="99"/>
+      <c r="A26" s="165" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="166"/>
+      <c r="C26" s="146" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="147"/>
+      <c r="E26" s="147"/>
+      <c r="F26" s="147"/>
+      <c r="G26" s="147"/>
+      <c r="H26" s="147"/>
+      <c r="I26" s="147"/>
+      <c r="J26" s="147"/>
+      <c r="K26" s="147"/>
+      <c r="L26" s="147"/>
+      <c r="M26" s="147"/>
+      <c r="N26" s="147"/>
+      <c r="O26" s="147"/>
+      <c r="P26" s="147"/>
+      <c r="Q26" s="147"/>
+      <c r="R26" s="147"/>
+      <c r="S26" s="148"/>
+      <c r="T26" s="191" t="s">
+        <v>61</v>
+      </c>
+      <c r="U26" s="192"/>
+      <c r="V26" s="205" t="s">
+        <v>61</v>
+      </c>
+      <c r="W26" s="206"/>
+      <c r="X26" s="206"/>
+      <c r="Y26" s="207"/>
+      <c r="Z26" s="184" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA26" s="212"/>
+      <c r="AB26" s="184" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC26" s="185"/>
+      <c r="AD26" s="213" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE26" s="214"/>
+      <c r="AF26" s="214"/>
+      <c r="AG26" s="214"/>
+      <c r="AH26" s="214"/>
+      <c r="AI26" s="214"/>
+      <c r="AJ26" s="214"/>
+      <c r="AK26" s="214"/>
+      <c r="AL26" s="214"/>
+      <c r="AM26" s="214"/>
+      <c r="AN26" s="214"/>
+      <c r="AO26" s="214"/>
+      <c r="AP26" s="214"/>
+      <c r="AQ26" s="215"/>
       <c r="AR26" s="22"/>
       <c r="AS26" s="21"/>
       <c r="AT26" s="21"/>
@@ -4376,73 +4340,73 @@
       <c r="AX26" s="21"/>
       <c r="AY26" s="20"/>
       <c r="AZ26" s="20"/>
-      <c r="BA26" s="114" t="s">
-        <v>61</v>
-      </c>
-      <c r="BB26" s="115"/>
-      <c r="BC26" s="116"/>
+      <c r="BA26" s="167" t="s">
+        <v>61</v>
+      </c>
+      <c r="BB26" s="168"/>
+      <c r="BC26" s="169"/>
       <c r="BD26" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:56" ht="24.5" customHeight="1">
-      <c r="A27" s="133" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="103"/>
-      <c r="C27" s="143" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="144"/>
-      <c r="E27" s="144"/>
-      <c r="F27" s="144"/>
-      <c r="G27" s="144"/>
-      <c r="H27" s="144"/>
-      <c r="I27" s="144"/>
-      <c r="J27" s="144"/>
-      <c r="K27" s="144"/>
-      <c r="L27" s="144"/>
-      <c r="M27" s="144"/>
-      <c r="N27" s="144"/>
-      <c r="O27" s="144"/>
-      <c r="P27" s="144"/>
-      <c r="Q27" s="144"/>
-      <c r="R27" s="144"/>
-      <c r="S27" s="145"/>
-      <c r="T27" s="112" t="s">
-        <v>61</v>
-      </c>
-      <c r="U27" s="113"/>
-      <c r="V27" s="172" t="s">
-        <v>61</v>
-      </c>
-      <c r="W27" s="173"/>
-      <c r="X27" s="173"/>
-      <c r="Y27" s="174"/>
-      <c r="Z27" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA27" s="103"/>
-      <c r="AB27" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC27" s="121"/>
-      <c r="AD27" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE27" s="95"/>
-      <c r="AF27" s="95"/>
-      <c r="AG27" s="95"/>
-      <c r="AH27" s="95"/>
-      <c r="AI27" s="95"/>
-      <c r="AJ27" s="95"/>
-      <c r="AK27" s="95"/>
-      <c r="AL27" s="95"/>
-      <c r="AM27" s="95"/>
-      <c r="AN27" s="95"/>
-      <c r="AO27" s="95"/>
-      <c r="AP27" s="95"/>
-      <c r="AQ27" s="96"/>
+      <c r="A27" s="136" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="137"/>
+      <c r="C27" s="186" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="187"/>
+      <c r="E27" s="187"/>
+      <c r="F27" s="187"/>
+      <c r="G27" s="187"/>
+      <c r="H27" s="187"/>
+      <c r="I27" s="187"/>
+      <c r="J27" s="187"/>
+      <c r="K27" s="187"/>
+      <c r="L27" s="187"/>
+      <c r="M27" s="187"/>
+      <c r="N27" s="187"/>
+      <c r="O27" s="187"/>
+      <c r="P27" s="187"/>
+      <c r="Q27" s="187"/>
+      <c r="R27" s="187"/>
+      <c r="S27" s="188"/>
+      <c r="T27" s="189" t="s">
+        <v>61</v>
+      </c>
+      <c r="U27" s="190"/>
+      <c r="V27" s="202" t="s">
+        <v>61</v>
+      </c>
+      <c r="W27" s="203"/>
+      <c r="X27" s="203"/>
+      <c r="Y27" s="204"/>
+      <c r="Z27" s="141" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA27" s="137"/>
+      <c r="AB27" s="141" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC27" s="142"/>
+      <c r="AD27" s="209" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE27" s="210"/>
+      <c r="AF27" s="210"/>
+      <c r="AG27" s="210"/>
+      <c r="AH27" s="210"/>
+      <c r="AI27" s="210"/>
+      <c r="AJ27" s="210"/>
+      <c r="AK27" s="210"/>
+      <c r="AL27" s="210"/>
+      <c r="AM27" s="210"/>
+      <c r="AN27" s="210"/>
+      <c r="AO27" s="210"/>
+      <c r="AP27" s="210"/>
+      <c r="AQ27" s="211"/>
       <c r="AR27" s="19"/>
       <c r="AS27" s="18"/>
       <c r="AT27" s="18"/>
@@ -4452,73 +4416,73 @@
       <c r="AX27" s="18"/>
       <c r="AY27" s="17"/>
       <c r="AZ27" s="17"/>
-      <c r="BA27" s="117" t="s">
-        <v>61</v>
-      </c>
-      <c r="BB27" s="118"/>
-      <c r="BC27" s="119"/>
+      <c r="BA27" s="138" t="s">
+        <v>61</v>
+      </c>
+      <c r="BB27" s="139"/>
+      <c r="BC27" s="140"/>
       <c r="BD27" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:56" ht="24.5" customHeight="1" thickBot="1">
-      <c r="A28" s="149" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="150"/>
-      <c r="C28" s="134" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="135"/>
-      <c r="E28" s="135"/>
-      <c r="F28" s="135"/>
-      <c r="G28" s="135"/>
-      <c r="H28" s="135"/>
-      <c r="I28" s="135"/>
-      <c r="J28" s="135"/>
-      <c r="K28" s="135"/>
-      <c r="L28" s="135"/>
-      <c r="M28" s="135"/>
-      <c r="N28" s="135"/>
-      <c r="O28" s="135"/>
-      <c r="P28" s="135"/>
-      <c r="Q28" s="135"/>
-      <c r="R28" s="135"/>
-      <c r="S28" s="136"/>
-      <c r="T28" s="110" t="s">
-        <v>61</v>
-      </c>
-      <c r="U28" s="111"/>
-      <c r="V28" s="222" t="s">
-        <v>61</v>
-      </c>
-      <c r="W28" s="223"/>
-      <c r="X28" s="223"/>
-      <c r="Y28" s="224"/>
-      <c r="Z28" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA28" s="101"/>
-      <c r="AB28" s="154" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC28" s="155"/>
-      <c r="AD28" s="97" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE28" s="98"/>
-      <c r="AF28" s="98"/>
-      <c r="AG28" s="98"/>
-      <c r="AH28" s="98"/>
-      <c r="AI28" s="98"/>
-      <c r="AJ28" s="98"/>
-      <c r="AK28" s="98"/>
-      <c r="AL28" s="98"/>
-      <c r="AM28" s="98"/>
-      <c r="AN28" s="98"/>
-      <c r="AO28" s="98"/>
-      <c r="AP28" s="98"/>
-      <c r="AQ28" s="99"/>
+      <c r="A28" s="158" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="159"/>
+      <c r="C28" s="146" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="147"/>
+      <c r="E28" s="147"/>
+      <c r="F28" s="147"/>
+      <c r="G28" s="147"/>
+      <c r="H28" s="147"/>
+      <c r="I28" s="147"/>
+      <c r="J28" s="147"/>
+      <c r="K28" s="147"/>
+      <c r="L28" s="147"/>
+      <c r="M28" s="147"/>
+      <c r="N28" s="147"/>
+      <c r="O28" s="147"/>
+      <c r="P28" s="147"/>
+      <c r="Q28" s="147"/>
+      <c r="R28" s="147"/>
+      <c r="S28" s="148"/>
+      <c r="T28" s="191" t="s">
+        <v>61</v>
+      </c>
+      <c r="U28" s="192"/>
+      <c r="V28" s="205" t="s">
+        <v>61</v>
+      </c>
+      <c r="W28" s="206"/>
+      <c r="X28" s="206"/>
+      <c r="Y28" s="207"/>
+      <c r="Z28" s="184" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA28" s="212"/>
+      <c r="AB28" s="163" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC28" s="164"/>
+      <c r="AD28" s="213" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE28" s="214"/>
+      <c r="AF28" s="214"/>
+      <c r="AG28" s="214"/>
+      <c r="AH28" s="214"/>
+      <c r="AI28" s="214"/>
+      <c r="AJ28" s="214"/>
+      <c r="AK28" s="214"/>
+      <c r="AL28" s="214"/>
+      <c r="AM28" s="214"/>
+      <c r="AN28" s="214"/>
+      <c r="AO28" s="214"/>
+      <c r="AP28" s="214"/>
+      <c r="AQ28" s="215"/>
       <c r="AR28" s="16"/>
       <c r="AS28" s="15"/>
       <c r="AT28" s="15"/>
@@ -4528,230 +4492,230 @@
       <c r="AX28" s="15"/>
       <c r="AY28" s="14"/>
       <c r="AZ28" s="14"/>
-      <c r="BA28" s="151" t="s">
-        <v>61</v>
-      </c>
-      <c r="BB28" s="152"/>
-      <c r="BC28" s="153"/>
+      <c r="BA28" s="160" t="s">
+        <v>61</v>
+      </c>
+      <c r="BB28" s="161"/>
+      <c r="BC28" s="162"/>
       <c r="BD28" s="13">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:56">
-      <c r="A29" s="156" t="s">
+    <row r="29" spans="1:56" ht="13" customHeight="1">
+      <c r="A29" s="170" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="157"/>
-      <c r="C29" s="157"/>
-      <c r="D29" s="157"/>
-      <c r="E29" s="157"/>
-      <c r="F29" s="157"/>
-      <c r="G29" s="157"/>
-      <c r="H29" s="157"/>
-      <c r="I29" s="157"/>
-      <c r="J29" s="157"/>
-      <c r="K29" s="157"/>
-      <c r="L29" s="157"/>
-      <c r="M29" s="157"/>
-      <c r="N29" s="157"/>
-      <c r="O29" s="157"/>
-      <c r="P29" s="157"/>
-      <c r="Q29" s="157"/>
-      <c r="R29" s="157"/>
-      <c r="S29" s="157"/>
-      <c r="T29" s="157"/>
-      <c r="U29" s="157"/>
-      <c r="V29" s="157"/>
-      <c r="W29" s="157"/>
-      <c r="X29" s="157"/>
-      <c r="Y29" s="157"/>
-      <c r="Z29" s="157"/>
-      <c r="AA29" s="157"/>
-      <c r="AB29" s="157"/>
-      <c r="AC29" s="157"/>
-      <c r="AD29" s="157"/>
-      <c r="AE29" s="157"/>
-      <c r="AF29" s="157"/>
-      <c r="AG29" s="158"/>
-      <c r="AH29" s="159">
+      <c r="B29" s="171"/>
+      <c r="C29" s="171"/>
+      <c r="D29" s="171"/>
+      <c r="E29" s="171"/>
+      <c r="F29" s="171"/>
+      <c r="G29" s="171"/>
+      <c r="H29" s="171"/>
+      <c r="I29" s="171"/>
+      <c r="J29" s="171"/>
+      <c r="K29" s="171"/>
+      <c r="L29" s="171"/>
+      <c r="M29" s="171"/>
+      <c r="N29" s="171"/>
+      <c r="O29" s="171"/>
+      <c r="P29" s="171"/>
+      <c r="Q29" s="171"/>
+      <c r="R29" s="171"/>
+      <c r="S29" s="171"/>
+      <c r="T29" s="171"/>
+      <c r="U29" s="171"/>
+      <c r="V29" s="171"/>
+      <c r="W29" s="171"/>
+      <c r="X29" s="171"/>
+      <c r="Y29" s="171"/>
+      <c r="Z29" s="171"/>
+      <c r="AA29" s="171"/>
+      <c r="AB29" s="171"/>
+      <c r="AC29" s="171"/>
+      <c r="AD29" s="171"/>
+      <c r="AE29" s="171"/>
+      <c r="AF29" s="171"/>
+      <c r="AG29" s="172"/>
+      <c r="AH29" s="173">
         <v>0</v>
       </c>
-      <c r="AI29" s="160"/>
-      <c r="AJ29" s="160"/>
-      <c r="AK29" s="160"/>
-      <c r="AL29" s="160"/>
-      <c r="AM29" s="160"/>
-      <c r="AN29" s="160"/>
-      <c r="AO29" s="160"/>
-      <c r="AP29" s="160"/>
-      <c r="AQ29" s="160"/>
-      <c r="AR29" s="160"/>
-      <c r="AS29" s="160"/>
-      <c r="AT29" s="160"/>
-      <c r="AU29" s="160"/>
-      <c r="AV29" s="160"/>
-      <c r="AW29" s="160"/>
-      <c r="AX29" s="160"/>
-      <c r="AY29" s="160"/>
-      <c r="AZ29" s="160"/>
-      <c r="BA29" s="160"/>
-      <c r="BB29" s="160"/>
-      <c r="BC29" s="161"/>
+      <c r="AI29" s="174"/>
+      <c r="AJ29" s="174"/>
+      <c r="AK29" s="174"/>
+      <c r="AL29" s="174"/>
+      <c r="AM29" s="174"/>
+      <c r="AN29" s="174"/>
+      <c r="AO29" s="174"/>
+      <c r="AP29" s="174"/>
+      <c r="AQ29" s="174"/>
+      <c r="AR29" s="174"/>
+      <c r="AS29" s="174"/>
+      <c r="AT29" s="174"/>
+      <c r="AU29" s="174"/>
+      <c r="AV29" s="174"/>
+      <c r="AW29" s="174"/>
+      <c r="AX29" s="174"/>
+      <c r="AY29" s="174"/>
+      <c r="AZ29" s="174"/>
+      <c r="BA29" s="174"/>
+      <c r="BB29" s="174"/>
+      <c r="BC29" s="175"/>
     </row>
-    <row r="30" spans="1:56">
-      <c r="A30" s="168" t="s">
+    <row r="30" spans="1:56" ht="13" customHeight="1">
+      <c r="A30" s="181" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="169"/>
-      <c r="C30" s="169"/>
-      <c r="D30" s="169"/>
-      <c r="E30" s="169"/>
-      <c r="F30" s="169"/>
-      <c r="G30" s="169"/>
-      <c r="H30" s="169"/>
-      <c r="I30" s="169"/>
-      <c r="J30" s="169"/>
-      <c r="K30" s="169"/>
-      <c r="L30" s="169"/>
-      <c r="M30" s="169"/>
-      <c r="N30" s="169"/>
-      <c r="O30" s="169"/>
-      <c r="P30" s="169"/>
-      <c r="Q30" s="169"/>
-      <c r="R30" s="169"/>
-      <c r="S30" s="169"/>
-      <c r="T30" s="169"/>
-      <c r="U30" s="169"/>
-      <c r="V30" s="169"/>
-      <c r="W30" s="169"/>
-      <c r="X30" s="169"/>
-      <c r="Y30" s="169"/>
-      <c r="Z30" s="169"/>
-      <c r="AA30" s="169"/>
-      <c r="AB30" s="169"/>
-      <c r="AC30" s="169"/>
-      <c r="AD30" s="169"/>
-      <c r="AE30" s="169"/>
-      <c r="AF30" s="169"/>
-      <c r="AG30" s="170"/>
-      <c r="AH30" s="162"/>
-      <c r="AI30" s="163"/>
-      <c r="AJ30" s="163"/>
-      <c r="AK30" s="163"/>
-      <c r="AL30" s="163"/>
-      <c r="AM30" s="163"/>
-      <c r="AN30" s="163"/>
-      <c r="AO30" s="163"/>
-      <c r="AP30" s="163"/>
-      <c r="AQ30" s="163"/>
-      <c r="AR30" s="163"/>
-      <c r="AS30" s="163"/>
-      <c r="AT30" s="163"/>
-      <c r="AU30" s="163"/>
-      <c r="AV30" s="163"/>
-      <c r="AW30" s="163"/>
-      <c r="AX30" s="163"/>
-      <c r="AY30" s="163"/>
-      <c r="AZ30" s="163"/>
-      <c r="BA30" s="163"/>
-      <c r="BB30" s="163"/>
-      <c r="BC30" s="164"/>
+      <c r="B30" s="182"/>
+      <c r="C30" s="182"/>
+      <c r="D30" s="182"/>
+      <c r="E30" s="182"/>
+      <c r="F30" s="182"/>
+      <c r="G30" s="182"/>
+      <c r="H30" s="182"/>
+      <c r="I30" s="182"/>
+      <c r="J30" s="182"/>
+      <c r="K30" s="182"/>
+      <c r="L30" s="182"/>
+      <c r="M30" s="182"/>
+      <c r="N30" s="182"/>
+      <c r="O30" s="182"/>
+      <c r="P30" s="182"/>
+      <c r="Q30" s="182"/>
+      <c r="R30" s="182"/>
+      <c r="S30" s="182"/>
+      <c r="T30" s="182"/>
+      <c r="U30" s="182"/>
+      <c r="V30" s="182"/>
+      <c r="W30" s="182"/>
+      <c r="X30" s="182"/>
+      <c r="Y30" s="182"/>
+      <c r="Z30" s="182"/>
+      <c r="AA30" s="182"/>
+      <c r="AB30" s="182"/>
+      <c r="AC30" s="182"/>
+      <c r="AD30" s="182"/>
+      <c r="AE30" s="182"/>
+      <c r="AF30" s="182"/>
+      <c r="AG30" s="183"/>
+      <c r="AH30" s="176"/>
+      <c r="AI30" s="224"/>
+      <c r="AJ30" s="224"/>
+      <c r="AK30" s="224"/>
+      <c r="AL30" s="224"/>
+      <c r="AM30" s="224"/>
+      <c r="AN30" s="224"/>
+      <c r="AO30" s="224"/>
+      <c r="AP30" s="224"/>
+      <c r="AQ30" s="224"/>
+      <c r="AR30" s="224"/>
+      <c r="AS30" s="224"/>
+      <c r="AT30" s="224"/>
+      <c r="AU30" s="224"/>
+      <c r="AV30" s="224"/>
+      <c r="AW30" s="224"/>
+      <c r="AX30" s="224"/>
+      <c r="AY30" s="224"/>
+      <c r="AZ30" s="224"/>
+      <c r="BA30" s="224"/>
+      <c r="BB30" s="224"/>
+      <c r="BC30" s="177"/>
     </row>
-    <row r="31" spans="1:56">
-      <c r="A31" s="168" t="s">
+    <row r="31" spans="1:56" ht="13" customHeight="1">
+      <c r="A31" s="181" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="169"/>
-      <c r="C31" s="169"/>
-      <c r="D31" s="169"/>
-      <c r="E31" s="169"/>
-      <c r="F31" s="169"/>
-      <c r="G31" s="169"/>
-      <c r="H31" s="169"/>
-      <c r="I31" s="169"/>
-      <c r="J31" s="169"/>
-      <c r="K31" s="169"/>
-      <c r="L31" s="169"/>
-      <c r="M31" s="169"/>
-      <c r="N31" s="169"/>
-      <c r="O31" s="169"/>
-      <c r="P31" s="169"/>
-      <c r="Q31" s="169"/>
-      <c r="R31" s="169"/>
-      <c r="S31" s="169"/>
-      <c r="T31" s="169"/>
-      <c r="U31" s="169"/>
-      <c r="V31" s="169"/>
-      <c r="W31" s="169"/>
-      <c r="X31" s="169"/>
-      <c r="Y31" s="169"/>
-      <c r="Z31" s="169"/>
-      <c r="AA31" s="169"/>
-      <c r="AB31" s="169"/>
-      <c r="AC31" s="169"/>
-      <c r="AD31" s="169"/>
-      <c r="AE31" s="169"/>
-      <c r="AF31" s="169"/>
-      <c r="AG31" s="170"/>
-      <c r="AH31" s="165"/>
-      <c r="AI31" s="166"/>
-      <c r="AJ31" s="166"/>
-      <c r="AK31" s="166"/>
-      <c r="AL31" s="166"/>
-      <c r="AM31" s="166"/>
-      <c r="AN31" s="166"/>
-      <c r="AO31" s="166"/>
-      <c r="AP31" s="166"/>
-      <c r="AQ31" s="166"/>
-      <c r="AR31" s="166"/>
-      <c r="AS31" s="166"/>
-      <c r="AT31" s="166"/>
-      <c r="AU31" s="166"/>
-      <c r="AV31" s="166"/>
-      <c r="AW31" s="166"/>
-      <c r="AX31" s="166"/>
-      <c r="AY31" s="166"/>
-      <c r="AZ31" s="166"/>
-      <c r="BA31" s="166"/>
-      <c r="BB31" s="166"/>
-      <c r="BC31" s="167"/>
+      <c r="B31" s="182"/>
+      <c r="C31" s="182"/>
+      <c r="D31" s="182"/>
+      <c r="E31" s="182"/>
+      <c r="F31" s="182"/>
+      <c r="G31" s="182"/>
+      <c r="H31" s="182"/>
+      <c r="I31" s="182"/>
+      <c r="J31" s="182"/>
+      <c r="K31" s="182"/>
+      <c r="L31" s="182"/>
+      <c r="M31" s="182"/>
+      <c r="N31" s="182"/>
+      <c r="O31" s="182"/>
+      <c r="P31" s="182"/>
+      <c r="Q31" s="182"/>
+      <c r="R31" s="182"/>
+      <c r="S31" s="182"/>
+      <c r="T31" s="182"/>
+      <c r="U31" s="182"/>
+      <c r="V31" s="182"/>
+      <c r="W31" s="182"/>
+      <c r="X31" s="182"/>
+      <c r="Y31" s="182"/>
+      <c r="Z31" s="182"/>
+      <c r="AA31" s="182"/>
+      <c r="AB31" s="182"/>
+      <c r="AC31" s="182"/>
+      <c r="AD31" s="182"/>
+      <c r="AE31" s="182"/>
+      <c r="AF31" s="182"/>
+      <c r="AG31" s="183"/>
+      <c r="AH31" s="178"/>
+      <c r="AI31" s="179"/>
+      <c r="AJ31" s="179"/>
+      <c r="AK31" s="179"/>
+      <c r="AL31" s="179"/>
+      <c r="AM31" s="179"/>
+      <c r="AN31" s="179"/>
+      <c r="AO31" s="179"/>
+      <c r="AP31" s="179"/>
+      <c r="AQ31" s="179"/>
+      <c r="AR31" s="179"/>
+      <c r="AS31" s="179"/>
+      <c r="AT31" s="179"/>
+      <c r="AU31" s="179"/>
+      <c r="AV31" s="179"/>
+      <c r="AW31" s="179"/>
+      <c r="AX31" s="179"/>
+      <c r="AY31" s="179"/>
+      <c r="AZ31" s="179"/>
+      <c r="BA31" s="179"/>
+      <c r="BB31" s="179"/>
+      <c r="BC31" s="180"/>
     </row>
     <row r="32" spans="1:56" ht="14" thickBot="1">
-      <c r="A32" s="146" t="s">
+      <c r="A32" s="155" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="147"/>
-      <c r="C32" s="147"/>
-      <c r="D32" s="147"/>
-      <c r="E32" s="147"/>
-      <c r="F32" s="147"/>
-      <c r="G32" s="147"/>
-      <c r="H32" s="147"/>
-      <c r="I32" s="147"/>
-      <c r="J32" s="147"/>
-      <c r="K32" s="147"/>
-      <c r="L32" s="147"/>
-      <c r="M32" s="147"/>
-      <c r="N32" s="147"/>
-      <c r="O32" s="147"/>
-      <c r="P32" s="147"/>
-      <c r="Q32" s="147"/>
-      <c r="R32" s="147"/>
-      <c r="S32" s="147"/>
-      <c r="T32" s="147"/>
-      <c r="U32" s="147"/>
-      <c r="V32" s="147"/>
-      <c r="W32" s="147"/>
-      <c r="X32" s="147"/>
-      <c r="Y32" s="147"/>
-      <c r="Z32" s="147"/>
-      <c r="AA32" s="147"/>
-      <c r="AB32" s="147"/>
-      <c r="AC32" s="147"/>
-      <c r="AD32" s="147"/>
-      <c r="AE32" s="147"/>
-      <c r="AF32" s="147"/>
-      <c r="AG32" s="148"/>
+      <c r="B32" s="156"/>
+      <c r="C32" s="156"/>
+      <c r="D32" s="156"/>
+      <c r="E32" s="156"/>
+      <c r="F32" s="156"/>
+      <c r="G32" s="156"/>
+      <c r="H32" s="156"/>
+      <c r="I32" s="156"/>
+      <c r="J32" s="156"/>
+      <c r="K32" s="156"/>
+      <c r="L32" s="156"/>
+      <c r="M32" s="156"/>
+      <c r="N32" s="156"/>
+      <c r="O32" s="156"/>
+      <c r="P32" s="156"/>
+      <c r="Q32" s="156"/>
+      <c r="R32" s="156"/>
+      <c r="S32" s="156"/>
+      <c r="T32" s="156"/>
+      <c r="U32" s="156"/>
+      <c r="V32" s="156"/>
+      <c r="W32" s="156"/>
+      <c r="X32" s="156"/>
+      <c r="Y32" s="156"/>
+      <c r="Z32" s="156"/>
+      <c r="AA32" s="156"/>
+      <c r="AB32" s="156"/>
+      <c r="AC32" s="156"/>
+      <c r="AD32" s="156"/>
+      <c r="AE32" s="156"/>
+      <c r="AF32" s="156"/>
+      <c r="AG32" s="157"/>
       <c r="AH32" s="12" t="s">
         <v>41</v>
       </c>
@@ -4779,45 +4743,50 @@
     </row>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="AA5:AN6"/>
-    <mergeCell ref="AO8:BC9"/>
-    <mergeCell ref="T11:AG13"/>
-    <mergeCell ref="AH11:AP13"/>
-    <mergeCell ref="AQ11:AW13"/>
-    <mergeCell ref="AX11:BC13"/>
-    <mergeCell ref="A5:Z5"/>
-    <mergeCell ref="A6:Z6"/>
-    <mergeCell ref="BB3:BC3"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="BA21:BC21"/>
-    <mergeCell ref="AB21:AC21"/>
-    <mergeCell ref="C19:S19"/>
-    <mergeCell ref="C20:S20"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:S18"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="A32:AG32"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="BA28:BC28"/>
-    <mergeCell ref="AB28:AC28"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="BA25:BC25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="BA26:BC26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="BA27:BC27"/>
-    <mergeCell ref="A29:AG29"/>
-    <mergeCell ref="AH29:BC31"/>
-    <mergeCell ref="A30:AG30"/>
-    <mergeCell ref="A31:AG31"/>
-    <mergeCell ref="AB26:AC26"/>
-    <mergeCell ref="AB27:AC27"/>
-    <mergeCell ref="AB25:AC25"/>
-    <mergeCell ref="C26:S26"/>
-    <mergeCell ref="C28:S28"/>
-    <mergeCell ref="C21:S21"/>
+    <mergeCell ref="Z28:AA28"/>
+    <mergeCell ref="AD20:AQ20"/>
+    <mergeCell ref="AD21:AQ21"/>
+    <mergeCell ref="AD22:AQ22"/>
+    <mergeCell ref="BA18:BC18"/>
+    <mergeCell ref="BA19:BC19"/>
+    <mergeCell ref="BA22:BC22"/>
+    <mergeCell ref="BA23:BC23"/>
+    <mergeCell ref="BA24:BC24"/>
+    <mergeCell ref="AR18:AZ18"/>
+    <mergeCell ref="BA20:BC20"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="AD26:AQ26"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="AB23:AC23"/>
+    <mergeCell ref="AB24:AC24"/>
+    <mergeCell ref="AD24:AQ24"/>
+    <mergeCell ref="AD25:AQ25"/>
+    <mergeCell ref="V22:Y22"/>
+    <mergeCell ref="V23:Y23"/>
+    <mergeCell ref="V24:Y24"/>
+    <mergeCell ref="V25:Y25"/>
+    <mergeCell ref="V26:Y26"/>
+    <mergeCell ref="Z26:AA26"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="AD23:AQ23"/>
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="T20:U20"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="AD19:AQ19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="AB20:AC20"/>
     <mergeCell ref="C23:S23"/>
     <mergeCell ref="C25:S25"/>
     <mergeCell ref="C27:S27"/>
@@ -4842,55 +4811,50 @@
     <mergeCell ref="V19:Y19"/>
     <mergeCell ref="Z19:AA19"/>
     <mergeCell ref="V20:Y20"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="T15:U15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="AD23:AQ23"/>
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="T20:U20"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="AD19:AQ19"/>
-    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="A32:AG32"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="BA28:BC28"/>
+    <mergeCell ref="AB28:AC28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="BA25:BC25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="BA26:BC26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="BA27:BC27"/>
+    <mergeCell ref="A29:AG29"/>
+    <mergeCell ref="AH29:BC31"/>
+    <mergeCell ref="A30:AG30"/>
+    <mergeCell ref="A31:AG31"/>
+    <mergeCell ref="AB26:AC26"/>
+    <mergeCell ref="AB27:AC27"/>
+    <mergeCell ref="AB25:AC25"/>
+    <mergeCell ref="C26:S26"/>
+    <mergeCell ref="C28:S28"/>
     <mergeCell ref="V28:Y28"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="Z21:AA21"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="AD26:AQ26"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="AB22:AC22"/>
-    <mergeCell ref="AB23:AC23"/>
-    <mergeCell ref="AB24:AC24"/>
-    <mergeCell ref="AD24:AQ24"/>
-    <mergeCell ref="AD25:AQ25"/>
-    <mergeCell ref="AB20:AC20"/>
-    <mergeCell ref="V22:Y22"/>
-    <mergeCell ref="V23:Y23"/>
-    <mergeCell ref="V24:Y24"/>
-    <mergeCell ref="V25:Y25"/>
-    <mergeCell ref="V26:Y26"/>
     <mergeCell ref="V27:Y27"/>
     <mergeCell ref="AD27:AQ27"/>
     <mergeCell ref="AD28:AQ28"/>
-    <mergeCell ref="Z26:AA26"/>
     <mergeCell ref="Z27:AA27"/>
-    <mergeCell ref="Z28:AA28"/>
-    <mergeCell ref="AD20:AQ20"/>
-    <mergeCell ref="AD21:AQ21"/>
-    <mergeCell ref="AD22:AQ22"/>
-    <mergeCell ref="BA18:BC18"/>
-    <mergeCell ref="BA19:BC19"/>
-    <mergeCell ref="BA22:BC22"/>
-    <mergeCell ref="BA23:BC23"/>
-    <mergeCell ref="BA24:BC24"/>
-    <mergeCell ref="AR18:AZ18"/>
-    <mergeCell ref="BA20:BC20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="BA21:BC21"/>
+    <mergeCell ref="AB21:AC21"/>
+    <mergeCell ref="C19:S19"/>
+    <mergeCell ref="C20:S20"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:S18"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="C21:S21"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="AA5:AN6"/>
+    <mergeCell ref="AO8:BC9"/>
+    <mergeCell ref="T11:AG13"/>
+    <mergeCell ref="AH11:AP13"/>
+    <mergeCell ref="AQ11:AW13"/>
+    <mergeCell ref="AX11:BC13"/>
+    <mergeCell ref="A5:Z5"/>
+    <mergeCell ref="A6:Z6"/>
+    <mergeCell ref="BB3:BC3"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>